<commit_message>
Styling, data update, hc.js local
Some styling updates, (including Open Sans fonts) and table update.
Also linking to local version of highcharts.js.
</commit_message>
<xml_diff>
--- a/raw-data/points-per-game.xlsx
+++ b/raw-data/points-per-game.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-160" yWindow="180" windowWidth="24620" windowHeight="16300" tabRatio="500"/>
+    <workbookView xWindow="2660" yWindow="1700" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Offense" sheetId="1" r:id="rId1"/>
     <sheet name="Defense" sheetId="2" r:id="rId2"/>
+    <sheet name="Super Bowl Winners" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="76">
   <si>
     <t>Team</t>
   </si>
@@ -122,12 +124,141 @@
   </si>
   <si>
     <t>Pts/G</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Winner</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Offense</t>
+  </si>
+  <si>
+    <t>Defense</t>
+  </si>
+  <si>
+    <t>XXXVII</t>
+  </si>
+  <si>
+    <t>48–21 vs Oakland Raiders</t>
+  </si>
+  <si>
+    <t>18th</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>XXXVIII</t>
+  </si>
+  <si>
+    <t>32–29 vs Carolina Panthers</t>
+  </si>
+  <si>
+    <t>12th</t>
+  </si>
+  <si>
+    <t>XXXIX</t>
+  </si>
+  <si>
+    <t>24–21 vs Philadelphia Eagles</t>
+  </si>
+  <si>
+    <t>4th</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>21–10 vs Seattle Seahawks</t>
+  </si>
+  <si>
+    <t>9th</t>
+  </si>
+  <si>
+    <t>3rd</t>
+  </si>
+  <si>
+    <t>XLI</t>
+  </si>
+  <si>
+    <t>29–17 vs Chicago Bears</t>
+  </si>
+  <si>
+    <t>23rd</t>
+  </si>
+  <si>
+    <t>XLII</t>
+  </si>
+  <si>
+    <t>17–14 vs New England Patriots</t>
+  </si>
+  <si>
+    <t>14th</t>
+  </si>
+  <si>
+    <t>17th</t>
+  </si>
+  <si>
+    <t>XLIII</t>
+  </si>
+  <si>
+    <t>27–23 vsArizona Cardinals</t>
+  </si>
+  <si>
+    <t>20th</t>
+  </si>
+  <si>
+    <t>XLIV</t>
+  </si>
+  <si>
+    <t>31–17 vs Indianapolis Colts</t>
+  </si>
+  <si>
+    <t>XLV</t>
+  </si>
+  <si>
+    <t>31–25 vs Pittsburgh Steelers</t>
+  </si>
+  <si>
+    <t>10th</t>
+  </si>
+  <si>
+    <t>XLVI</t>
+  </si>
+  <si>
+    <t>21–17 vs New England Patriots</t>
+  </si>
+  <si>
+    <t>25th</t>
+  </si>
+  <si>
+    <t>XLVII</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>at New Orleans, Louisiana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -185,12 +316,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3235,4 +3367,280 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5">
+        <v>37647</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="5">
+        <v>38018</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="5">
+        <v>38389</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="5">
+        <v>38753</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="5">
+        <v>39117</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="5">
+        <v>39481</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="5">
+        <v>39845</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="5">
+        <v>40216</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="5">
+        <v>40580</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="5">
+        <v>40944</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="5">
+        <v>41308</v>
+      </c>
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>